<commit_message>
initial commit to net
</commit_message>
<xml_diff>
--- a/Reference Template.xlsx
+++ b/Reference Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niall.McSharry\OneDrive - Department of Health and Social Care\Documents\Git\BoldDHSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthsharedservice-my.sharepoint.com/personal/niall_mcsharry_dhsc_gov_uk/Documents/Documents/Git/BoldDHSC/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{23207CFE-4E04-4386-8B99-8CA99B29511F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
@@ -139,12 +139,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{28DE8D95-B390-4729-BE72-9603749CC30E}" name="Table2" displayName="Table2" ref="A1:C2" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{28DE8D95-B390-4729-BE72-9603749CC30E}" name="Table2" displayName="Table2" ref="A1:C2" totalsRowShown="0" dataDxfId="3">
   <autoFilter ref="A1:C2" xr:uid="{28DE8D95-B390-4729-BE72-9603749CC30E}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{CBACC272-0F1F-43EF-A033-E1E74DCEC7B6}" name="Variable_name" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{4049B00D-7ED2-43F7-8161-BBA9CC2145EC}" name="Variable_type" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{DB947455-D941-4911-91AA-691A8DF0A6AF}" name="Variable_description" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{CBACC272-0F1F-43EF-A033-E1E74DCEC7B6}" name="Variable_name" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{4049B00D-7ED2-43F7-8161-BBA9CC2145EC}" name="Variable_type" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{DB947455-D941-4911-91AA-691A8DF0A6AF}" name="Variable_description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -482,7 +482,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>